<commit_message>
Fix curly brace replacement
</commit_message>
<xml_diff>
--- a/Source/Amba.Report.Test/Amba.Report.Test/Templates/Orders2.xlsx
+++ b/Source/Amba.Report.Test/Amba.Report.Test/Templates/Orders2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="36210" yWindow="120" windowWidth="23775" windowHeight="15015"/>
+    <workbookView xWindow="38070" yWindow="120" windowWidth="23775" windowHeight="15015"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="3" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <t>Company: {Company.Name}</t>
   </si>
   <si>
-    <t>Report date: {Date: MMM dd, yyyy}</t>
+    <t>Report date: {Date:dd.MM.yyyy}</t>
   </si>
 </sst>
 </file>
@@ -223,6 +223,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -256,7 +257,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -634,11 +634,11 @@
       <c r="B4" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
@@ -647,29 +647,29 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="15">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="6">
         <v>0</v>
       </c>
@@ -678,11 +678,11 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="7">
         <v>0</v>
       </c>
@@ -691,11 +691,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="8">
         <v>0</v>
       </c>
@@ -707,8 +707,8 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
@@ -716,7 +716,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>